<commit_message>
updated start scrip and fixed user upload issue
</commit_message>
<xml_diff>
--- a/host/instance/uploads/Users_file.xlsx
+++ b/host/instance/uploads/Users_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mackenziefurlong/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51549A9-B84F-9145-9065-2389026047C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8540E6-3C45-4644-84C3-2DDF8382671B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="480" windowWidth="25600" windowHeight="14140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>userID</t>
   </si>
@@ -50,9 +50,6 @@
   </si>
   <si>
     <t>michael</t>
-  </si>
-  <si>
-    <t>12345</t>
   </si>
   <si>
     <t>Graham Gibson</t>
@@ -429,7 +426,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -470,26 +467,26 @@
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
       <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -497,28 +494,28 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>18</v>
-      </c>
-      <c r="I3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -526,28 +523,28 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H4">
         <v>24</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated start script and fixed upload users error
</commit_message>
<xml_diff>
--- a/host/instance/uploads/Users_file.xlsx
+++ b/host/instance/uploads/Users_file.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mackenziefurlong/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Graham\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51549A9-B84F-9145-9065-2389026047C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7DA4D9F-DD80-498F-9A00-D40FCC2B0027}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="25600" windowHeight="14140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>userID</t>
   </si>
@@ -49,43 +49,34 @@
     <t>Permissions</t>
   </si>
   <si>
-    <t>michael</t>
-  </si>
-  <si>
-    <t>12345</t>
-  </si>
-  <si>
-    <t>Graham Gibson</t>
-  </si>
-  <si>
-    <t>Queen's University</t>
-  </si>
-  <si>
-    <t>CMC</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>1010101</t>
-  </si>
-  <si>
-    <t>Mackenzie</t>
-  </si>
-  <si>
-    <t>42132</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>1111111</t>
-  </si>
-  <si>
-    <t>joe</t>
-  </si>
-  <si>
-    <t>0111011</t>
+    <t>0010010</t>
+  </si>
+  <si>
+    <t>George McFly</t>
+  </si>
+  <si>
+    <t>Doc Brown</t>
+  </si>
+  <si>
+    <t>Chemistry</t>
+  </si>
+  <si>
+    <t>ArtSci</t>
+  </si>
+  <si>
+    <t>Queen's</t>
+  </si>
+  <si>
+    <t>Marty McFly</t>
+  </si>
+  <si>
+    <t>0100011</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>Academic Machine Dependent</t>
   </si>
 </sst>
 </file>
@@ -426,15 +417,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -463,15 +458,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
         <v>10</v>
+      </c>
+      <c r="C2">
+        <v>13</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -483,24 +478,24 @@
         <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3">
         <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -512,42 +507,13 @@
         <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4">
-        <v>24</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>21</v>
+      <c r="I3" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed issue with receiving leading zero in permissions leading to edit user error
</commit_message>
<xml_diff>
--- a/host/instance/uploads/Users_file.xlsx
+++ b/host/instance/uploads/Users_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mackenziefurlong/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8540E6-3C45-4644-84C3-2DDF8382671B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BF738A7-B707-F741-A08B-361FF33E0184}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="480" windowWidth="25600" windowHeight="14140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
   <si>
     <t>userID</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t>0111011</t>
+  </si>
+  <si>
+    <t>24</t>
   </si>
 </sst>
 </file>
@@ -426,7 +429,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -540,8 +543,8 @@
       <c r="G4" t="s">
         <v>12</v>
       </c>
-      <c r="H4">
-        <v>24</v>
+      <c r="H4" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>20</v>

</xml_diff>